<commit_message>
push sebelum revisi terakhir part3?
</commit_message>
<xml_diff>
--- a/COretan.xlsx
+++ b/COretan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8E7E92-19FB-4B9A-8EC2-A21F299627A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0484659C-6D3F-4E8D-B91D-CD303A1AA54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="1488" windowWidth="17280" windowHeight="8880" xr2:uid="{7A1AF197-6D99-47DD-86E4-115774CD5D11}"/>
+    <workbookView visibility="hidden" minimized="1" xWindow="2940" yWindow="2352" windowWidth="17280" windowHeight="8880" xr2:uid="{7A1AF197-6D99-47DD-86E4-115774CD5D11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Konversi Satuan Berat</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Item 2</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot;Rp&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;Rp&quot;#,##0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -202,12 +205,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1856EA93-A26E-4562-AC10-42AE796C3044}">
-  <dimension ref="F2:K23"/>
+  <dimension ref="F2:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,11 +540,12 @@
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G2">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="6:11" x14ac:dyDescent="0.3">
@@ -555,11 +559,11 @@
     <row r="4" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F4">
         <f>G2*G3%</f>
-        <v>59.18</v>
+        <v>58.74</v>
       </c>
       <c r="G4">
         <f>G2*H3%</f>
-        <v>209.82</v>
+        <v>208.26000000000002</v>
       </c>
     </row>
     <row r="5" spans="6:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -590,7 +594,7 @@
       <c r="I6" s="8">
         <v>750000</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="10">
         <v>200000</v>
       </c>
     </row>
@@ -600,7 +604,7 @@
       </c>
       <c r="G7">
         <f>ROUND(G4,0)</f>
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H7">
         <v>0.75</v>
@@ -608,7 +612,7 @@
       <c r="I7" s="7">
         <v>100000</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F8" s="1"/>
@@ -621,7 +625,7 @@
         <f>G6*H6</f>
         <v>29.5</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="6" t="s">
@@ -636,7 +640,7 @@
         <f>(G9/1000) * I6</f>
         <v>22125</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I10" s="6" t="s">
@@ -651,7 +655,7 @@
         <f>J6/G9</f>
         <v>6779.6610169491523</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -664,9 +668,9 @@
       </c>
       <c r="G12">
         <f>G7*H7</f>
-        <v>157.5</v>
-      </c>
-      <c r="H12" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="6" t="s">
@@ -679,9 +683,9 @@
       </c>
       <c r="G13" s="7">
         <f>(G12/1000) * I6</f>
-        <v>118125</v>
-      </c>
-      <c r="H13" s="10" t="s">
+        <v>117000</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I13" s="6" t="s">
@@ -694,9 +698,9 @@
       </c>
       <c r="G14" s="7">
         <f>J6/G12</f>
-        <v>1269.8412698412699</v>
-      </c>
-      <c r="H14" s="10" t="s">
+        <v>1282.051282051282</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="6" t="s">
@@ -711,7 +715,7 @@
         <f>SQRT((2*G9*(G10+I7))/(J6/G9))</f>
         <v>32.60050325531801</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="I15">
@@ -732,24 +736,24 @@
       </c>
       <c r="G16">
         <f>SQRT((2*G12*(G13+I7))/(J6/G12))</f>
-        <v>232.61262393193539</v>
-      </c>
-      <c r="H16" s="10" t="s">
+        <v>229.80234985743726</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>12</v>
       </c>
       <c r="I16">
         <f>ROUND(G16,0)</f>
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="K16">
         <f>I16/H7</f>
-        <v>310.66666666666669</v>
-      </c>
-    </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+        <v>306.66666666666669</v>
+      </c>
+    </row>
+    <row r="18" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
         <v>8</v>
       </c>
@@ -758,8 +762,19 @@
         <v>80.789077232012005</v>
       </c>
     </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:17" x14ac:dyDescent="0.3">
       <c r="H23" s="2"/>
+    </row>
+    <row r="25" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="Q25" s="7">
+        <f>267*20000</f>
+        <v>5340000</v>
+      </c>
+    </row>
+    <row r="26" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="P26" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>